<commit_message>
Custom PNL updates to meet the project requirements
Updates to the Excel graph templates (style changes only). The template
for the commercial team is now being auto-populated. There is still work
to do around inputting ICP numbers and setting the custom date for YTD
calcs.
</commit_message>
<xml_diff>
--- a/Data/Templates.xlsx
+++ b/Data/Templates.xlsx
@@ -4,17 +4,172 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Rob" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Would be ([YTD target] - [previous month's YTD target]) for all months other than April.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Would be ([YTD target] - [previous month's YTD target]) for all months other than April.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Would be ([YTD target] - [previous month's YTD target]) for all months other than April.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Would be ([YTD target] - [previous month's YTD target]) for all months other than April.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Would be ([YTD target] - [previous month's YTD target]) for all months other than April.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Would be ([YTD target] - [previous month's YTD target]) for all months other than April.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
   <si>
     <t>key_NETWORK_NAME</t>
   </si>
@@ -104,13 +259,199 @@
   </si>
   <si>
     <t>key_DATE</t>
+  </si>
+  <si>
+    <t>Electricity Invercargill</t>
+  </si>
+  <si>
+    <t>Operational Performance</t>
+  </si>
+  <si>
+    <t>YTD</t>
+  </si>
+  <si>
+    <t>Full Year Forecast</t>
+  </si>
+  <si>
+    <t>Full Year Target</t>
+  </si>
+  <si>
+    <t>YTD Figures as at</t>
+  </si>
+  <si>
+    <t>Reliability Target - mid ComCom target</t>
+  </si>
+  <si>
+    <t>- Planned</t>
+  </si>
+  <si>
+    <t>- Unplanned Normalised</t>
+  </si>
+  <si>
+    <t>- Total assessed against target</t>
+  </si>
+  <si>
+    <t>YTD SAIDI Cap</t>
+  </si>
+  <si>
+    <t>- Projected Incentive/Penalty</t>
+  </si>
+  <si>
+    <t>YTD SAIDI Collar</t>
+  </si>
+  <si>
+    <t>YTD SAIFI Cap</t>
+  </si>
+  <si>
+    <t>YTD SAIFI Collar</t>
+  </si>
+  <si>
+    <t>The Power Company</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>OtagoNet</t>
+  </si>
+  <si>
+    <t>Normalised Out SAIDI</t>
+  </si>
+  <si>
+    <t>Normalised Out SAIFI</t>
+  </si>
+  <si>
+    <r>
+      <t>SAIDI</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IR</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SAIFI</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IR</t>
+    </r>
+  </si>
+  <si>
+    <t>key_EIL_CUST_NUM</t>
+  </si>
+  <si>
+    <t>key_TPC_CUST_NUM</t>
+  </si>
+  <si>
+    <t>key_OJV_CUST_NUM</t>
+  </si>
+  <si>
+    <t>key_EIL_SAIDI_PLANNED</t>
+  </si>
+  <si>
+    <t>key_EIL_SAIDI_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_EIL_SAIFI_PLANNED</t>
+  </si>
+  <si>
+    <t>key_EIL_SAIFI_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_TPC_SAIDI_PLANNED</t>
+  </si>
+  <si>
+    <t>key_TPC_SAIDI_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_TPC_SAIFI_PLANNED</t>
+  </si>
+  <si>
+    <t>key_TPC_SAIFI_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_OJV_SAIDI_PLANNED</t>
+  </si>
+  <si>
+    <t>key_OJV_SAIDI_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_OJV_SAIFI_PLANNED</t>
+  </si>
+  <si>
+    <t>key_OJV_SAIFI_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_EIL_CC_SAIDI_YTD</t>
+  </si>
+  <si>
+    <t>key_EIL_CC_SAIFI_YTD</t>
+  </si>
+  <si>
+    <t>key_TPC_CC_SAIDI_YTD</t>
+  </si>
+  <si>
+    <t>key_TPC_CC_SAIFI_YTD</t>
+  </si>
+  <si>
+    <t>key_OJV_CC_SAIDI_YTD</t>
+  </si>
+  <si>
+    <t>key_OJV_CC_SAIFI_YTD</t>
+  </si>
+  <si>
+    <t>key_EIL_DATE_END</t>
+  </si>
+  <si>
+    <t>key_EIL_SAIDI_NORMED_OUT</t>
+  </si>
+  <si>
+    <t>key_TPC_SAIDI_NORMED_OUT</t>
+  </si>
+  <si>
+    <t>key_TPC_SAIFI_NORMED_OUT</t>
+  </si>
+  <si>
+    <t>key_OJV_SAIDI_NORMED_OUT</t>
+  </si>
+  <si>
+    <t>key_OJV_SAIFI_NORMED_OUT</t>
+  </si>
+  <si>
+    <t>key_EIL_SAIFI_NORMED_OUT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="6">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,16 +475,72 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -295,15 +692,211 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -327,14 +920,120 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma 2" xfId="2"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -636,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,181 +1350,181 @@
     <col min="10" max="10" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
         <v>9</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="16" t="s">
+      <c r="I3" s="10"/>
+      <c r="J3" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="13" t="s">
+      <c r="I4" s="8"/>
+      <c r="J4" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="13" t="s">
+      <c r="I5" s="8"/>
+      <c r="J5" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="5"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -833,4 +1532,1008 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="10" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="55"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="37">
+        <f>1%*13565*1000</f>
+        <v>135650</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="34"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="34">
+        <f>SUM(F5:F6)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="35"/>
+      <c r="I7" s="38" t="e">
+        <f>F7-G7+J7</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J7" s="45">
+        <v>24.075885772705</v>
+      </c>
+      <c r="K7" s="39"/>
+      <c r="L7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="1">
+        <v>31.126729965209901</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="41" t="e">
+        <f>IF(I7&lt;M8, M5/2, IF(I7&gt;M7, -M5/2, (J7-I7)*M9))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="1">
+        <v>17.025041580200099</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="43"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="50">
+        <f>0.5*M5/(M7-J7)</f>
+        <v>9619.415512272768</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="33"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="45"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="33"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="38"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.77168273925781194</v>
+      </c>
+      <c r="O11" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="38">
+        <f>SUM(F10:F11)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="48"/>
+      <c r="I12" s="38" t="e">
+        <f>F12-G12+J12</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J12" s="45">
+        <v>0.59350174665451005</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.41532078385353099</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="41" t="e">
+        <f>IF(I12&lt;M12, M5/2, IF(I12&gt;M11, -M5/2, (J12-I12)*M13))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G13" s="34"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="M13" s="50">
+        <f>0.5*M5/(M11-J12)</f>
+        <v>380652.2738988442</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="55"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="34"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="34"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="33"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="34">
+        <f>SUM(F19:F20)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="35"/>
+      <c r="I21" s="34" t="e">
+        <f>F21-G21+J21</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J21" s="45">
+        <v>150.02806000000001</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M21" s="1">
+        <v>165.66626439250879</v>
+      </c>
+      <c r="O21" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="33"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="41" t="e">
+        <f>IF(I21&lt;M22, M19/2, IF(I21&gt;M21, -M19/2, (J21-I21)*M23))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G22" s="34"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M22" s="1">
+        <v>134.38985400061679</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="43"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M23" s="50" t="e">
+        <f>0.5*M19/(M21-J21)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="33"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="45"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="33"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="45"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M25" s="1">
+        <v>3.1582358015733725</v>
+      </c>
+      <c r="O25" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="33"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="45">
+        <f>SUM(F24:F25)</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" s="46"/>
+      <c r="I26" s="45" t="e">
+        <f>F26-G26+J26</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J26" s="45">
+        <v>2.8460200000000002</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M26" s="1">
+        <v>2.5337967140967539</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A27" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="41" t="e">
+        <f>IF(I26&lt;M26, M19/2, IF(I26&gt;M25, -M19/2, (J26-I26)*M27))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="M27" s="50" t="e">
+        <f>0.5*M19/(M25-J26)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="18"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H31" s="21"/>
+      <c r="I31" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K31" s="1"/>
+      <c r="L31" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="M31" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="J32" s="55"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="33"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="34"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M33" s="37">
+        <f>1%*24780*1000</f>
+        <v>247800</v>
+      </c>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="33"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="34"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="33"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="34">
+        <f>SUM(F33:F34)</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="H35" s="35"/>
+      <c r="I35" s="34" t="e">
+        <f>F35-G35+J35</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J35" s="45">
+        <v>224.57734680175699</v>
+      </c>
+      <c r="K35" s="1"/>
+      <c r="L35" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M35" s="1">
+        <v>254.91531372070301</v>
+      </c>
+      <c r="O35" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="33"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="41" t="e">
+        <f>IF(I35&lt;M36, M33/2, IF(I35&gt;M35, -M33/2, (J35-I35)*M37))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G36" s="34"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M36" s="1">
+        <v>194.23937988281199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A37" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="43"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M37" s="37">
+        <f>0.5*M33/(M35-J35)</f>
+        <v>4083.9915321624471</v>
+      </c>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="33"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="45"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="O38" s="1"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="33"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" s="45"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M39" s="1">
+        <v>2.9273090362548801</v>
+      </c>
+      <c r="O39" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="33"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="45">
+        <f>SUM(F38:F39)</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="H40" s="46"/>
+      <c r="I40" s="45" t="e">
+        <f>F40-G40+J40</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J40" s="47">
+        <v>2.5238583087921098</v>
+      </c>
+      <c r="K40" s="1"/>
+      <c r="L40" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M40" s="1">
+        <v>2.1204075813293399</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="33"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="41" t="e">
+        <f>IF(I40&lt;M40, M33/2, IF(I40&gt;M39, -M33/2, (J40-I40)*M41))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G41" s="34"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="36"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="M41" s="37">
+        <f>0.5*M33/(M39-J40)</f>
+        <v>307100.69796920434</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I32:J32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added by month reporting to the commercial team's template
Also, added the values to populate the new dictionary keys in Output.py
</commit_message>
<xml_diff>
--- a/Data/Templates.xlsx
+++ b/Data/Templates.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="102">
   <si>
     <t>key_NETWORK_NAME</t>
   </si>
@@ -438,13 +438,80 @@
   <si>
     <t>key_EIL_SAIFI_NORMED_OUT</t>
   </si>
+  <si>
+    <t>key_EIL_SAIDI_MONTH_PLANNED</t>
+  </si>
+  <si>
+    <t>key_EIL_SAIDI_MONTH_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_TPC_SAIDI_MONTH_PLANNED</t>
+  </si>
+  <si>
+    <t>key_TPC_SAIDI_MONTH_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_OJV_SAIDI_MONTH_PLANNED</t>
+  </si>
+  <si>
+    <t>key_OJV_SAIDI_MONTH_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_EIL_SAIFI_MONTH_PLANNED</t>
+  </si>
+  <si>
+    <t>key_EIL_SAIFI_MONTH_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_TPC_SAIFI_MONTH_PLANNED</t>
+  </si>
+  <si>
+    <t>key_TPC_SAIFI_MONTH_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_OJV_SAIFI_MONTH_PLANNED</t>
+  </si>
+  <si>
+    <t>key_OJV_SAIFI_MONTH_UNPLANNED</t>
+  </si>
+  <si>
+    <t>Normalised Out SAIDI (Month)</t>
+  </si>
+  <si>
+    <t>Normalised Out SAIFI (Month)</t>
+  </si>
+  <si>
+    <t>key_EIL_SAIDI_MONTH_NORMED_OUT</t>
+  </si>
+  <si>
+    <t>key_EIL_SAIFI_MONTH_NORMED_OUT</t>
+  </si>
+  <si>
+    <t>key_TPC_SAIDI_MONTH_NORMED_OUT</t>
+  </si>
+  <si>
+    <t>key_TPC_SAIFI_MONTH_NORMED_OUT</t>
+  </si>
+  <si>
+    <t>key_OJV_SAIDI_MONTH_NORMED_OUT</t>
+  </si>
+  <si>
+    <t>key_OJV_SAIFI_MONTH_NORMED_OUT</t>
+  </si>
+  <si>
+    <t>End of Month Target</t>
+  </si>
+  <si>
+    <t>Month to Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -895,7 +962,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1015,6 +1082,9 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1359,18 +1429,18 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -1539,17 +1609,20 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="10" width="19.28515625" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1582,8 +1655,12 @@
         <v>31</v>
       </c>
       <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
+      <c r="C3" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>100</v>
+      </c>
       <c r="E3" s="21"/>
       <c r="F3" s="22" t="s">
         <v>32</v>
@@ -1617,10 +1694,10 @@
       <c r="F4" s="28"/>
       <c r="G4" s="29"/>
       <c r="H4" s="31"/>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="55"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="1"/>
       <c r="L4" s="16" t="s">
         <v>26</v>
@@ -1634,7 +1711,9 @@
         <v>37</v>
       </c>
       <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
+      <c r="C5" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="D5" s="34"/>
       <c r="E5" s="35"/>
       <c r="F5" s="34" t="s">
@@ -1658,7 +1737,9 @@
         <v>38</v>
       </c>
       <c r="B6" s="33"/>
-      <c r="C6" s="34"/>
+      <c r="C6" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="D6" s="34"/>
       <c r="E6" s="35"/>
       <c r="F6" s="34" t="s">
@@ -1677,8 +1758,14 @@
         <v>39</v>
       </c>
       <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+      <c r="C7" s="34">
+        <f>SUM(C5:C6)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="51">
+        <f>J7/12</f>
+        <v>2.0063238143920832</v>
+      </c>
       <c r="E7" s="35"/>
       <c r="F7" s="34">
         <f>SUM(F5:F6)</f>
@@ -1731,6 +1818,12 @@
       </c>
       <c r="M8" s="1">
         <v>17.025041580200099</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -1760,7 +1853,9 @@
         <v>37</v>
       </c>
       <c r="B10" s="33"/>
-      <c r="C10" s="45"/>
+      <c r="C10" s="34" t="s">
+        <v>86</v>
+      </c>
       <c r="D10" s="45"/>
       <c r="E10" s="46"/>
       <c r="F10" s="34" t="s">
@@ -1779,7 +1874,9 @@
         <v>38</v>
       </c>
       <c r="B11" s="33"/>
-      <c r="C11" s="45"/>
+      <c r="C11" s="34" t="s">
+        <v>87</v>
+      </c>
       <c r="D11" s="45"/>
       <c r="E11" s="46"/>
       <c r="F11" s="34" t="s">
@@ -1808,8 +1905,14 @@
         <v>39</v>
       </c>
       <c r="B12" s="33"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
+      <c r="C12" s="34">
+        <f>SUM(C10:C11)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="51">
+        <f>J12/12</f>
+        <v>4.9458478887875836E-2</v>
+      </c>
       <c r="E12" s="46"/>
       <c r="F12" s="38">
         <f>SUM(F10:F11)</f>
@@ -1832,6 +1935,12 @@
       </c>
       <c r="M12" s="1">
         <v>0.41532078385353099</v>
+      </c>
+      <c r="O12" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -1911,8 +2020,12 @@
         <v>31</v>
       </c>
       <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>100</v>
+      </c>
       <c r="E17" s="21"/>
       <c r="F17" s="22" t="s">
         <v>32</v>
@@ -1947,10 +2060,10 @@
       <c r="F18" s="28"/>
       <c r="G18" s="29"/>
       <c r="H18" s="31"/>
-      <c r="I18" s="54" t="s">
+      <c r="I18" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="55"/>
+      <c r="J18" s="56"/>
       <c r="K18" s="1"/>
       <c r="L18" s="16" t="s">
         <v>26</v>
@@ -1965,7 +2078,9 @@
         <v>37</v>
       </c>
       <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
+      <c r="C19" s="34" t="s">
+        <v>82</v>
+      </c>
       <c r="D19" s="34"/>
       <c r="E19" s="35"/>
       <c r="F19" s="34" t="s">
@@ -1989,7 +2104,9 @@
         <v>38</v>
       </c>
       <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
+      <c r="C20" s="34" t="s">
+        <v>83</v>
+      </c>
       <c r="D20" s="34"/>
       <c r="E20" s="35"/>
       <c r="F20" s="34" t="s">
@@ -2008,8 +2125,14 @@
         <v>39</v>
       </c>
       <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
+      <c r="C21" s="34">
+        <f>SUM(C19:C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="51">
+        <f>J21/12</f>
+        <v>12.502338333333334</v>
+      </c>
       <c r="E21" s="35"/>
       <c r="F21" s="34">
         <f>SUM(F19:F20)</f>
@@ -2062,6 +2185,12 @@
       </c>
       <c r="M22" s="1">
         <v>134.38985400061679</v>
+      </c>
+      <c r="O22" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -2092,7 +2221,9 @@
         <v>37</v>
       </c>
       <c r="B24" s="33"/>
-      <c r="C24" s="45"/>
+      <c r="C24" s="34" t="s">
+        <v>88</v>
+      </c>
       <c r="D24" s="45"/>
       <c r="E24" s="46"/>
       <c r="F24" s="34" t="s">
@@ -2112,7 +2243,9 @@
         <v>38</v>
       </c>
       <c r="B25" s="33"/>
-      <c r="C25" s="45"/>
+      <c r="C25" s="34" t="s">
+        <v>89</v>
+      </c>
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
       <c r="F25" s="34" t="s">
@@ -2141,8 +2274,14 @@
         <v>39</v>
       </c>
       <c r="B26" s="33"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
+      <c r="C26" s="34">
+        <f>SUM(C24:C25)</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="45">
+        <f>J26/12</f>
+        <v>0.23716833333333334</v>
+      </c>
       <c r="E26" s="46"/>
       <c r="F26" s="45">
         <f>SUM(F24:F25)</f>
@@ -2165,6 +2304,12 @@
       </c>
       <c r="M26" s="1">
         <v>2.5337967140967539</v>
+      </c>
+      <c r="O26" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -2244,8 +2389,12 @@
         <v>31</v>
       </c>
       <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20"/>
+      <c r="C31" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>100</v>
+      </c>
       <c r="E31" s="21"/>
       <c r="F31" s="22" t="s">
         <v>32</v>
@@ -2280,10 +2429,10 @@
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
       <c r="H32" s="31"/>
-      <c r="I32" s="54" t="s">
+      <c r="I32" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="J32" s="55"/>
+      <c r="J32" s="56"/>
       <c r="K32" s="1"/>
       <c r="L32" s="16" t="s">
         <v>26</v>
@@ -2298,7 +2447,9 @@
         <v>37</v>
       </c>
       <c r="B33" s="33"/>
-      <c r="C33" s="34"/>
+      <c r="C33" s="34" t="s">
+        <v>84</v>
+      </c>
       <c r="D33" s="34"/>
       <c r="E33" s="35"/>
       <c r="F33" s="34" t="s">
@@ -2323,7 +2474,9 @@
         <v>38</v>
       </c>
       <c r="B34" s="33"/>
-      <c r="C34" s="34"/>
+      <c r="C34" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="D34" s="34"/>
       <c r="E34" s="35"/>
       <c r="F34" s="34" t="s">
@@ -2342,8 +2495,14 @@
         <v>39</v>
       </c>
       <c r="B35" s="33"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
+      <c r="C35" s="34">
+        <f>SUM(C33:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="51">
+        <f>J35/12</f>
+        <v>18.714778900146417</v>
+      </c>
       <c r="E35" s="35"/>
       <c r="F35" s="34">
         <f>SUM(F33:F34)</f>
@@ -2396,6 +2555,12 @@
       </c>
       <c r="M36" s="1">
         <v>194.23937988281199</v>
+      </c>
+      <c r="O36" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -2426,7 +2591,9 @@
         <v>37</v>
       </c>
       <c r="B38" s="33"/>
-      <c r="C38" s="45"/>
+      <c r="C38" s="34" t="s">
+        <v>90</v>
+      </c>
       <c r="D38" s="45"/>
       <c r="E38" s="46"/>
       <c r="F38" s="34" t="s">
@@ -2446,7 +2613,9 @@
         <v>38</v>
       </c>
       <c r="B39" s="33"/>
-      <c r="C39" s="45"/>
+      <c r="C39" s="34" t="s">
+        <v>91</v>
+      </c>
       <c r="D39" s="45"/>
       <c r="E39" s="46"/>
       <c r="F39" s="34" t="s">
@@ -2475,8 +2644,14 @@
         <v>39</v>
       </c>
       <c r="B40" s="33"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
+      <c r="C40" s="34">
+        <f>SUM(C38:C39)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="45">
+        <f>J40/12</f>
+        <v>0.21032152573267582</v>
+      </c>
       <c r="E40" s="46"/>
       <c r="F40" s="45">
         <f>SUM(F38:F39)</f>
@@ -2499,6 +2674,12 @@
       </c>
       <c r="M40" s="1">
         <v>2.1204075813293399</v>
+      </c>
+      <c r="O40" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="18" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added extra report values to the template report for the Commercial Team
</commit_message>
<xml_diff>
--- a/Data/Templates.xlsx
+++ b/Data/Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -68,30 +68,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Would be ([YTD target] - [previous month's YTD target]) for all months other than April.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="D26" authorId="0">
       <text>
         <r>
@@ -116,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D35" authorId="0">
+    <comment ref="D31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +116,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D40" authorId="0">
+    <comment ref="D45" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Would be ([YTD target] - [previous month's YTD target]) for all months other than April.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D50" authorId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="133">
   <si>
     <t>key_NETWORK_NAME</t>
   </si>
@@ -503,6 +503,99 @@
   </si>
   <si>
     <t>Month to Date</t>
+  </si>
+  <si>
+    <t>Raw</t>
+  </si>
+  <si>
+    <t>- Number of Unplanned Faults</t>
+  </si>
+  <si>
+    <t>- Number of Planned Faults</t>
+  </si>
+  <si>
+    <t>key_EIL_RAW_MONTH_PLANNED</t>
+  </si>
+  <si>
+    <t>key_EIL_RAW_PLANNED</t>
+  </si>
+  <si>
+    <t>key_EIL_RAW_MONTH_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_EIL_RAW_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_TPC_RAW_MONTH_PLANNED</t>
+  </si>
+  <si>
+    <t>key_TPC_RAW_MONTH_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_TPC_RAW_PLANNED</t>
+  </si>
+  <si>
+    <t>key_TPC_RAW_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_OJV_RAW_MONTH_PLANNED</t>
+  </si>
+  <si>
+    <t>key_OJV_RAW_MONTH_UNPLANNED</t>
+  </si>
+  <si>
+    <t>key_OJV_RAW_PLANNED</t>
+  </si>
+  <si>
+    <t>key_OJV_RAW_UNPLANNED</t>
+  </si>
+  <si>
+    <t>- Number of Major Event Days (SAIFI)</t>
+  </si>
+  <si>
+    <t>- Number of Major Event Days (SAIDI)</t>
+  </si>
+  <si>
+    <t>key_EIL_RAW_MONTH_NUM_MAJOR_EVENTS_SAIFI</t>
+  </si>
+  <si>
+    <t>key_EIL_RAW_MONTH_NUM_MAJOR_EVENTS_SAIDI</t>
+  </si>
+  <si>
+    <t>key_EIL_RAW_NUM_MAJOR_EVENTS_SAIDI</t>
+  </si>
+  <si>
+    <t>key_EIL_RAW_NUM_MAJOR_EVENTS_SAIFI</t>
+  </si>
+  <si>
+    <t>key_TPC_RAW_MONTH_NUM_MAJOR_EVENTS_SAIDI</t>
+  </si>
+  <si>
+    <t>key_TPC_RAW_MONTH_NUM_MAJOR_EVENTS_SAIFI</t>
+  </si>
+  <si>
+    <t>key_TPC_RAW_NUM_MAJOR_EVENTS_SAIDI</t>
+  </si>
+  <si>
+    <t>key_TPC_RAW_NUM_MAJOR_EVENTS_SAIFI</t>
+  </si>
+  <si>
+    <t>key_OJV_RAW_MONTH_NUM_MAJOR_EVENTS_SAIDI</t>
+  </si>
+  <si>
+    <t>key_OJV_RAW_MONTH_NUM_MAJOR_EVENTS_SAIFI</t>
+  </si>
+  <si>
+    <t>key_OJV_RAW_NUM_MAJOR_EVENTS_SAIDI</t>
+  </si>
+  <si>
+    <t>key_OJV_RAW_NUM_MAJOR_EVENTS_SAIFI</t>
+  </si>
+  <si>
+    <t>SAIDI (Average Outage Minutes/ICP)</t>
+  </si>
+  <si>
+    <t>SAIFI (Average Number of Interruptions/ICP)</t>
   </si>
 </sst>
 </file>
@@ -962,7 +1055,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1083,6 +1176,9 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1429,18 +1525,18 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -1606,15 +1702,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
@@ -1627,7 +1723,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1">
         <v>16</v>
@@ -1685,7 +1781,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="28"/>
@@ -1694,10 +1790,10 @@
       <c r="F4" s="28"/>
       <c r="G4" s="29"/>
       <c r="H4" s="31"/>
-      <c r="I4" s="55" t="s">
+      <c r="I4" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="56"/>
+      <c r="J4" s="57"/>
       <c r="K4" s="1"/>
       <c r="L4" s="16" t="s">
         <v>26</v>
@@ -1828,7 +1924,7 @@
     </row>
     <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="42" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="34"/>
@@ -1968,251 +2064,204 @@
         <v>380652.2738988442</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="21"/>
-      <c r="I17" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="L17" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="M17" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="J18" s="56"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O18" s="1"/>
+    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="43"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="36"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="50"/>
+    </row>
+    <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="33"/>
+      <c r="C15" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="45"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" s="45"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="47"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="50"/>
+    </row>
+    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="45"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="52" t="s">
+        <v>108</v>
+      </c>
+      <c r="G16" s="45"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="47"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="50"/>
+    </row>
+    <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="45"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="G17" s="45"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="47"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="50"/>
+    </row>
+    <row r="18" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="G18" s="45"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="47"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="50"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="36"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="36"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34">
-        <f>SUM(C19:C20)</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="51">
-        <f>J21/12</f>
-        <v>12.502338333333334</v>
-      </c>
-      <c r="E21" s="35"/>
-      <c r="F21" s="34">
-        <f>SUM(F19:F20)</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" s="35"/>
-      <c r="I21" s="34" t="e">
-        <f>F21-G21+J21</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J21" s="45">
-        <v>150.02806000000001</v>
-      </c>
+    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M21" s="1">
-        <v>165.66626439250879</v>
-      </c>
-      <c r="O21" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="41" t="e">
-        <f>IF(I21&lt;M22, M19/2, IF(I21&gt;M21, -M19/2, (J21-I21)*M23))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="K22" s="1"/>
       <c r="L22" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="M22" s="1">
-        <v>134.38985400061679</v>
-      </c>
-      <c r="O22" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="36"/>
+        <v>35</v>
+      </c>
+      <c r="M22" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="57"/>
       <c r="K23" s="1"/>
       <c r="L23" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="M23" s="50" t="e">
-        <f>0.5*M19/(M21-J21)</f>
-        <v>#VALUE!</v>
+        <v>26</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="O23" s="1"/>
     </row>
@@ -2222,20 +2271,24 @@
       </c>
       <c r="B24" s="33"/>
       <c r="C24" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="45"/>
-      <c r="E24" s="46"/>
+        <v>82</v>
+      </c>
+      <c r="D24" s="34"/>
+      <c r="E24" s="35"/>
       <c r="F24" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="G24" s="45"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="47"/>
+        <v>59</v>
+      </c>
+      <c r="G24" s="34"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="36"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="L24" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="O24" s="1"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -2244,30 +2297,20 @@
       </c>
       <c r="B25" s="33"/>
       <c r="C25" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="45"/>
-      <c r="E25" s="46"/>
+        <v>83</v>
+      </c>
+      <c r="D25" s="34"/>
+      <c r="E25" s="35"/>
       <c r="F25" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" s="45"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="47"/>
+        <v>60</v>
+      </c>
+      <c r="G25" s="34"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="36"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M25" s="1">
-        <v>3.1582358015733725</v>
-      </c>
-      <c r="O25" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
@@ -2278,440 +2321,771 @@
         <f>SUM(C24:C25)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="45">
+      <c r="D26" s="51">
         <f>J26/12</f>
-        <v>0.23716833333333334</v>
-      </c>
-      <c r="E26" s="46"/>
-      <c r="F26" s="45">
+        <v>12.502338333333334</v>
+      </c>
+      <c r="E26" s="35"/>
+      <c r="F26" s="34">
         <f>SUM(F24:F25)</f>
         <v>0</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="H26" s="46"/>
-      <c r="I26" s="45" t="e">
+        <v>69</v>
+      </c>
+      <c r="H26" s="35"/>
+      <c r="I26" s="34" t="e">
         <f>F26-G26+J26</f>
         <v>#VALUE!</v>
       </c>
       <c r="J26" s="45">
-        <v>2.8460200000000002</v>
+        <v>150.02806000000001</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M26" s="1">
-        <v>2.5337967140967539</v>
+        <v>165.66626439250879</v>
       </c>
       <c r="O26" s="16" t="s">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B27" s="33"/>
       <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
+      <c r="D27" s="40"/>
       <c r="E27" s="35"/>
       <c r="F27" s="41" t="e">
-        <f>IF(I26&lt;M26, M19/2, IF(I26&gt;M25, -M19/2, (J26-I26)*M27))</f>
+        <f>IF(I26&lt;M27, M24/2, IF(I26&gt;M26, -M24/2, (J26-I26)*M28))</f>
         <v>#VALUE!</v>
       </c>
       <c r="G27" s="34"/>
       <c r="H27" s="35"/>
       <c r="I27" s="34"/>
-      <c r="J27" s="36"/>
+      <c r="J27" s="34"/>
       <c r="K27" s="1"/>
       <c r="L27" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="M27" s="50" t="e">
-        <f>0.5*M19/(M25-J26)</f>
+        <v>3</v>
+      </c>
+      <c r="M27" s="1">
+        <v>134.38985400061679</v>
+      </c>
+      <c r="O27" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M28" s="50" t="e">
+        <f>0.5*M24/(M26-J26)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="O28" s="1"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="39"/>
+      <c r="A29" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="33"/>
+      <c r="C29" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="45"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" s="45"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="47"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="33"/>
+      <c r="C30" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="45"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="45"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="47"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="J31" s="24" t="s">
-        <v>34</v>
+      <c r="L30" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M30" s="1">
+        <v>3.1582358015733725</v>
+      </c>
+      <c r="O30" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="33"/>
+      <c r="C31" s="34">
+        <f>SUM(C29:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="45">
+        <f>J31/12</f>
+        <v>0.23716833333333334</v>
+      </c>
+      <c r="E31" s="46"/>
+      <c r="F31" s="45">
+        <f>SUM(F29:F30)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="H31" s="46"/>
+      <c r="I31" s="45" t="e">
+        <f>F31-G31+J31</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J31" s="45">
+        <v>2.8460200000000002</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="M31" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="O31" s="1"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="J32" s="56"/>
+        <v>3</v>
+      </c>
+      <c r="M31" s="1">
+        <v>2.5337967140967539</v>
+      </c>
+      <c r="O31" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A32" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="41" t="e">
+        <f>IF(I31&lt;M31, M24/2, IF(I31&gt;M30, -M24/2, (J31-I31)*M32))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G32" s="34"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="36"/>
       <c r="K32" s="1"/>
       <c r="L32" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="O32" s="1"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D33" s="34"/>
+        <v>51</v>
+      </c>
+      <c r="M32" s="50" t="e">
+        <f>0.5*M24/(M30-J31)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="43"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="44"/>
       <c r="E33" s="35"/>
-      <c r="F33" s="34" t="s">
-        <v>63</v>
-      </c>
+      <c r="F33" s="34"/>
       <c r="G33" s="34"/>
       <c r="H33" s="35"/>
       <c r="I33" s="34"/>
       <c r="J33" s="36"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="M33" s="37">
-        <f>1%*24780*1000</f>
-        <v>247800</v>
-      </c>
-      <c r="O33" s="1"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L33" s="16"/>
+      <c r="M33" s="50"/>
+    </row>
+    <row r="34" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="B34" s="33"/>
-      <c r="C34" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="34"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C34" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="45"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="G34" s="45"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="47"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="50"/>
+    </row>
+    <row r="35" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="B35" s="33"/>
-      <c r="C35" s="34">
-        <f>SUM(C33:C34)</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="51">
-        <f>J35/12</f>
-        <v>18.714778900146417</v>
-      </c>
-      <c r="E35" s="35"/>
-      <c r="F35" s="34">
-        <f>SUM(F33:F34)</f>
-        <v>0</v>
-      </c>
-      <c r="G35" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="H35" s="35"/>
-      <c r="I35" s="34" t="e">
-        <f>F35-G35+J35</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J35" s="45">
-        <v>224.57734680175699</v>
-      </c>
-      <c r="K35" s="1"/>
-      <c r="L35" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M35" s="1">
-        <v>254.91531372070301</v>
-      </c>
-      <c r="O35" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C35" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="45"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="G35" s="45"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="47"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="50"/>
+    </row>
+    <row r="36" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="B36" s="33"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="41" t="e">
-        <f>IF(I35&lt;M36, M33/2, IF(I35&gt;M35, -M33/2, (J35-I35)*M37))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G36" s="34"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="M36" s="1">
-        <v>194.23937988281199</v>
-      </c>
-      <c r="O36" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="18" x14ac:dyDescent="0.35">
-      <c r="A37" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="43"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="M37" s="37">
-        <f>0.5*M33/(M35-J35)</f>
-        <v>4083.9915321624471</v>
-      </c>
-      <c r="O37" s="1"/>
+      <c r="C36" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="45"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="G36" s="45"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="47"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="50"/>
+    </row>
+    <row r="37" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37" s="33"/>
+      <c r="C37" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" s="45"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="G37" s="45"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="47"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="50"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="33"/>
-      <c r="C38" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="D38" s="45"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="G38" s="45"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="47"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
-      <c r="O38" s="1"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="33"/>
-      <c r="C39" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="D39" s="45"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="G39" s="45"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="47"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="39"/>
       <c r="K39" s="1"/>
-      <c r="L39" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M39" s="1">
-        <v>2.9273090362548801</v>
-      </c>
-      <c r="O39" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="34">
-        <f>SUM(C38:C39)</f>
-        <v>0</v>
-      </c>
-      <c r="D40" s="45">
-        <f>J40/12</f>
-        <v>0.21032152573267582</v>
-      </c>
-      <c r="E40" s="46"/>
-      <c r="F40" s="45">
-        <f>SUM(F38:F39)</f>
-        <v>0</v>
-      </c>
-      <c r="G40" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="H40" s="46"/>
-      <c r="I40" s="45" t="e">
-        <f>F40-G40+J40</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J40" s="47">
-        <v>2.5238583087921098</v>
-      </c>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-      <c r="L40" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="M40" s="1">
-        <v>2.1204075813293399</v>
-      </c>
-      <c r="O40" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="18" x14ac:dyDescent="0.35">
-      <c r="A41" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="41" t="e">
-        <f>IF(I40&lt;M40, M33/2, IF(I40&gt;M39, -M33/2, (J40-I40)*M41))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G41" s="34"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="36"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="18"/>
+      <c r="C41" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" s="21"/>
+      <c r="F41" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="21"/>
+      <c r="I41" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J41" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="K41" s="1"/>
       <c r="L41" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="M41" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="O41" s="1"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" s="27"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="J42" s="57"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O42" s="1"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="33"/>
+      <c r="C43" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" s="34"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="G43" s="34"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M43" s="37">
+        <f>1%*24780*1000</f>
+        <v>247800</v>
+      </c>
+      <c r="O43" s="1"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="33"/>
+      <c r="C44" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="34"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" s="34"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="36"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="33"/>
+      <c r="C45" s="34">
+        <f>SUM(C43:C44)</f>
+        <v>0</v>
+      </c>
+      <c r="D45" s="51">
+        <f>J45/12</f>
+        <v>18.714778900146417</v>
+      </c>
+      <c r="E45" s="35"/>
+      <c r="F45" s="34">
+        <f>SUM(F43:F44)</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="H45" s="35"/>
+      <c r="I45" s="34" t="e">
+        <f>F45-G45+J45</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J45" s="45">
+        <v>224.57734680175699</v>
+      </c>
+      <c r="K45" s="1"/>
+      <c r="L45" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M45" s="1">
+        <v>254.91531372070301</v>
+      </c>
+      <c r="O45" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="33"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="41" t="e">
+        <f>IF(I45&lt;M46, M43/2, IF(I45&gt;M45, -M43/2, (J45-I45)*M47))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G46" s="34"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M46" s="1">
+        <v>194.23937988281199</v>
+      </c>
+      <c r="O46" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A47" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B47" s="43"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="36"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M47" s="37">
+        <f>0.5*M43/(M45-J45)</f>
+        <v>4083.9915321624471</v>
+      </c>
+      <c r="O47" s="1"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="33"/>
+      <c r="C48" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" s="45"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="45"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="47"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="O48" s="1"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="33"/>
+      <c r="C49" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D49" s="45"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="G49" s="45"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="47"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M49" s="1">
+        <v>2.9273090362548801</v>
+      </c>
+      <c r="O49" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="33"/>
+      <c r="C50" s="34">
+        <f>SUM(C48:C49)</f>
+        <v>0</v>
+      </c>
+      <c r="D50" s="45">
+        <f>J50/12</f>
+        <v>0.21032152573267582</v>
+      </c>
+      <c r="E50" s="46"/>
+      <c r="F50" s="45">
+        <f>SUM(F48:F49)</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="H50" s="46"/>
+      <c r="I50" s="45" t="e">
+        <f>F50-G50+J50</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J50" s="47">
+        <v>2.5238583087921098</v>
+      </c>
+      <c r="K50" s="1"/>
+      <c r="L50" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M50" s="1">
+        <v>2.1204075813293399</v>
+      </c>
+      <c r="O50" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A51" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="33"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="41" t="e">
+        <f>IF(I50&lt;M50, M43/2, IF(I50&gt;M49, -M43/2, (J50-I50)*M51))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G51" s="34"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="34"/>
+      <c r="J51" s="36"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="M41" s="37">
-        <f>0.5*M33/(M39-J40)</f>
+      <c r="M51" s="37">
+        <f>0.5*M43/(M49-J50)</f>
         <v>307100.69796920434</v>
       </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="43"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="36"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="33"/>
+      <c r="C53" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="45"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="G53" s="45"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="45"/>
+      <c r="J53" s="47"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="33"/>
+      <c r="C54" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="45"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="G54" s="45"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="47"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" s="33"/>
+      <c r="C55" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="D55" s="45"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="G55" s="45"/>
+      <c r="H55" s="46"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="47"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="33"/>
+      <c r="C56" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="D56" s="45"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="G56" s="45"/>
+      <c r="H56" s="46"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I42:J42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes to formatting to make the output KPI compliant
Also made it so that the console boxes close themselves after a short
delay
</commit_message>
<xml_diff>
--- a/Data/Templates.xlsx
+++ b/Data/Templates.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="27795" windowHeight="12405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="132">
   <si>
     <t>key_NETWORK_NAME</t>
   </si>
@@ -307,9 +307,6 @@
   </si>
   <si>
     <t>The Power Company</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>OtagoNet</t>
@@ -1055,7 +1052,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1196,6 +1193,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 2" xfId="2"/>
@@ -1705,7 +1703,7 @@
   <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,10 +1750,10 @@
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="22" t="s">
@@ -1776,12 +1774,12 @@
         <v>35</v>
       </c>
       <c r="M3" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="28"/>
@@ -1799,7 +1797,7 @@
         <v>26</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1808,12 +1806,12 @@
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="35"/>
       <c r="F5" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="34"/>
       <c r="H5" s="35"/>
@@ -1834,12 +1832,12 @@
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="35"/>
       <c r="F6" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="35"/>
@@ -1868,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H7" s="35"/>
       <c r="I7" s="38" t="e">
@@ -1886,10 +1884,10 @@
         <v>31.126729965209901</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1916,15 +1914,15 @@
         <v>17.025041580200099</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="34"/>
@@ -1937,7 +1935,7 @@
       <c r="J9" s="36"/>
       <c r="K9" s="1"/>
       <c r="L9" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M9" s="50">
         <f>0.5*M5/(M7-J7)</f>
@@ -1950,12 +1948,12 @@
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="45"/>
       <c r="E10" s="46"/>
       <c r="F10" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10" s="45"/>
       <c r="H10" s="46"/>
@@ -1971,12 +1969,12 @@
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="45"/>
       <c r="E11" s="46"/>
       <c r="F11" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G11" s="38"/>
       <c r="H11" s="48"/>
@@ -1990,10 +1988,10 @@
         <v>0.77168273925781194</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2015,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" s="48"/>
       <c r="I12" s="38" t="e">
@@ -2033,10 +2031,10 @@
         <v>0.41532078385353099</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -2057,7 +2055,7 @@
       <c r="J13" s="36"/>
       <c r="K13" s="1"/>
       <c r="L13" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M13" s="50">
         <f>0.5*M5/(M11-J12)</f>
@@ -2066,7 +2064,7 @@
     </row>
     <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B14" s="43"/>
       <c r="C14" s="34"/>
@@ -2082,16 +2080,16 @@
     </row>
     <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="52" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="46"/>
       <c r="F15" s="52" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G15" s="45"/>
       <c r="H15" s="46"/>
@@ -2102,16 +2100,16 @@
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="46"/>
       <c r="F16" s="52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G16" s="45"/>
       <c r="H16" s="46"/>
@@ -2122,16 +2120,16 @@
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="46"/>
       <c r="F17" s="52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G17" s="45"/>
       <c r="H17" s="46"/>
@@ -2142,16 +2140,16 @@
     </row>
     <row r="18" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D18" s="45"/>
       <c r="E18" s="46"/>
       <c r="F18" s="52" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G18" s="45"/>
       <c r="H18" s="46"/>
@@ -2213,10 +2211,10 @@
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E22" s="21"/>
       <c r="F22" s="22" t="s">
@@ -2237,13 +2235,13 @@
         <v>35</v>
       </c>
       <c r="M22" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -2261,7 +2259,7 @@
         <v>26</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O23" s="1"/>
     </row>
@@ -2271,12 +2269,12 @@
       </c>
       <c r="B24" s="33"/>
       <c r="C24" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" s="34"/>
       <c r="E24" s="35"/>
       <c r="F24" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G24" s="34"/>
       <c r="H24" s="35"/>
@@ -2286,8 +2284,8 @@
       <c r="L24" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>46</v>
+      <c r="M24" s="58">
+        <v>438977</v>
       </c>
       <c r="O24" s="1"/>
     </row>
@@ -2297,12 +2295,12 @@
       </c>
       <c r="B25" s="33"/>
       <c r="C25" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D25" s="34"/>
       <c r="E25" s="35"/>
       <c r="F25" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G25" s="34"/>
       <c r="H25" s="35"/>
@@ -2331,7 +2329,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H26" s="35"/>
       <c r="I26" s="34" t="e">
@@ -2349,10 +2347,10 @@
         <v>165.66626439250879</v>
       </c>
       <c r="O26" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -2379,15 +2377,15 @@
         <v>134.38985400061679</v>
       </c>
       <c r="O27" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B28" s="43"/>
       <c r="C28" s="34"/>
@@ -2400,11 +2398,11 @@
       <c r="J28" s="36"/>
       <c r="K28" s="1"/>
       <c r="L28" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="M28" s="50" t="e">
+        <v>49</v>
+      </c>
+      <c r="M28" s="50">
         <f>0.5*M24/(M26-J26)</f>
-        <v>#VALUE!</v>
+        <v>14035.402945950895</v>
       </c>
       <c r="O28" s="1"/>
     </row>
@@ -2414,12 +2412,12 @@
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="46"/>
       <c r="F29" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G29" s="45"/>
       <c r="H29" s="46"/>
@@ -2436,12 +2434,12 @@
       </c>
       <c r="B30" s="33"/>
       <c r="C30" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="46"/>
       <c r="F30" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G30" s="45"/>
       <c r="H30" s="46"/>
@@ -2455,10 +2453,10 @@
         <v>3.1582358015733725</v>
       </c>
       <c r="O30" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2480,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H31" s="46"/>
       <c r="I31" s="45" t="e">
@@ -2498,10 +2496,10 @@
         <v>2.5337967140967539</v>
       </c>
       <c r="O31" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -2522,16 +2520,16 @@
       <c r="J32" s="36"/>
       <c r="K32" s="1"/>
       <c r="L32" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="M32" s="50" t="e">
+        <v>50</v>
+      </c>
+      <c r="M32" s="50">
         <f>0.5*M24/(M30-J31)</f>
-        <v>#VALUE!</v>
+        <v>703002.53508603771</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B33" s="43"/>
       <c r="C33" s="34"/>
@@ -2547,16 +2545,16 @@
     </row>
     <row r="34" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B34" s="33"/>
       <c r="C34" s="52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D34" s="45"/>
       <c r="E34" s="46"/>
       <c r="F34" s="52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G34" s="45"/>
       <c r="H34" s="46"/>
@@ -2567,16 +2565,16 @@
     </row>
     <row r="35" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B35" s="33"/>
       <c r="C35" s="52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="46"/>
       <c r="F35" s="52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G35" s="45"/>
       <c r="H35" s="46"/>
@@ -2587,16 +2585,16 @@
     </row>
     <row r="36" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B36" s="33"/>
       <c r="C36" s="52" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D36" s="45"/>
       <c r="E36" s="46"/>
       <c r="F36" s="52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G36" s="45"/>
       <c r="H36" s="46"/>
@@ -2607,16 +2605,16 @@
     </row>
     <row r="37" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B37" s="33"/>
       <c r="C37" s="52" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D37" s="45"/>
       <c r="E37" s="46"/>
       <c r="F37" s="52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G37" s="45"/>
       <c r="H37" s="46"/>
@@ -2657,7 +2655,7 @@
     </row>
     <row r="40" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2678,10 +2676,10 @@
       </c>
       <c r="B41" s="18"/>
       <c r="C41" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E41" s="21"/>
       <c r="F41" s="22" t="s">
@@ -2702,13 +2700,13 @@
         <v>35</v>
       </c>
       <c r="M41" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O41" s="1"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B42" s="27"/>
       <c r="C42" s="28"/>
@@ -2726,7 +2724,7 @@
         <v>26</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O42" s="1"/>
     </row>
@@ -2736,12 +2734,12 @@
       </c>
       <c r="B43" s="33"/>
       <c r="C43" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D43" s="34"/>
       <c r="E43" s="35"/>
       <c r="F43" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G43" s="34"/>
       <c r="H43" s="35"/>
@@ -2763,12 +2761,12 @@
       </c>
       <c r="B44" s="33"/>
       <c r="C44" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44" s="34"/>
       <c r="E44" s="35"/>
       <c r="F44" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G44" s="34"/>
       <c r="H44" s="35"/>
@@ -2797,7 +2795,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H45" s="35"/>
       <c r="I45" s="34" t="e">
@@ -2815,10 +2813,10 @@
         <v>254.91531372070301</v>
       </c>
       <c r="O45" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -2845,15 +2843,15 @@
         <v>194.23937988281199</v>
       </c>
       <c r="O46" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B47" s="43"/>
       <c r="C47" s="34"/>
@@ -2866,7 +2864,7 @@
       <c r="J47" s="36"/>
       <c r="K47" s="1"/>
       <c r="L47" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M47" s="37">
         <f>0.5*M43/(M45-J45)</f>
@@ -2880,12 +2878,12 @@
       </c>
       <c r="B48" s="33"/>
       <c r="C48" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D48" s="45"/>
       <c r="E48" s="46"/>
       <c r="F48" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G48" s="45"/>
       <c r="H48" s="46"/>
@@ -2902,12 +2900,12 @@
       </c>
       <c r="B49" s="33"/>
       <c r="C49" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D49" s="45"/>
       <c r="E49" s="46"/>
       <c r="F49" s="34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G49" s="45"/>
       <c r="H49" s="46"/>
@@ -2921,10 +2919,10 @@
         <v>2.9273090362548801</v>
       </c>
       <c r="O49" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -2946,7 +2944,7 @@
         <v>0</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H50" s="46"/>
       <c r="I50" s="45" t="e">
@@ -2964,10 +2962,10 @@
         <v>2.1204075813293399</v>
       </c>
       <c r="O50" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -2988,7 +2986,7 @@
       <c r="J51" s="36"/>
       <c r="K51" s="1"/>
       <c r="L51" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M51" s="37">
         <f>0.5*M43/(M49-J50)</f>
@@ -2997,7 +2995,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B52" s="43"/>
       <c r="C52" s="34"/>
@@ -3011,16 +3009,16 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B53" s="33"/>
       <c r="C53" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D53" s="45"/>
       <c r="E53" s="46"/>
       <c r="F53" s="52" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G53" s="45"/>
       <c r="H53" s="46"/>
@@ -3029,16 +3027,16 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="33"/>
       <c r="C54" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D54" s="45"/>
       <c r="E54" s="46"/>
       <c r="F54" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G54" s="45"/>
       <c r="H54" s="46"/>
@@ -3047,16 +3045,16 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B55" s="33"/>
       <c r="C55" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D55" s="45"/>
       <c r="E55" s="46"/>
       <c r="F55" s="52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G55" s="45"/>
       <c r="H55" s="46"/>
@@ -3065,16 +3063,16 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B56" s="33"/>
       <c r="C56" s="52" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D56" s="45"/>
       <c r="E56" s="46"/>
       <c r="F56" s="52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G56" s="45"/>
       <c r="H56" s="46"/>

</xml_diff>

<commit_message>
Updates to limit the precission in the UBV, and other ComCom table variables
</commit_message>
<xml_diff>
--- a/Data/Templates.xlsx
+++ b/Data/Templates.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Rob" sheetId="2" r:id="rId2"/>
+    <sheet name="Commercial" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -1178,6 +1178,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1193,7 +1194,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 2" xfId="2"/>
@@ -1523,18 +1523,18 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="56"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -1788,10 +1788,10 @@
       <c r="F4" s="28"/>
       <c r="G4" s="29"/>
       <c r="H4" s="31"/>
-      <c r="I4" s="56" t="s">
+      <c r="I4" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="57"/>
+      <c r="J4" s="58"/>
       <c r="K4" s="1"/>
       <c r="L4" s="16" t="s">
         <v>26</v>
@@ -2250,10 +2250,10 @@
       <c r="F23" s="28"/>
       <c r="G23" s="29"/>
       <c r="H23" s="31"/>
-      <c r="I23" s="56" t="s">
+      <c r="I23" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="J23" s="57"/>
+      <c r="J23" s="58"/>
       <c r="K23" s="1"/>
       <c r="L23" s="16" t="s">
         <v>26</v>
@@ -2284,7 +2284,7 @@
       <c r="L24" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="M24" s="58">
+      <c r="M24" s="53">
         <v>438977</v>
       </c>
       <c r="O24" s="1"/>
@@ -2715,10 +2715,10 @@
       <c r="F42" s="28"/>
       <c r="G42" s="29"/>
       <c r="H42" s="31"/>
-      <c r="I42" s="56" t="s">
+      <c r="I42" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="J42" s="57"/>
+      <c r="J42" s="58"/>
       <c r="K42" s="1"/>
       <c r="L42" s="16" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Replaced and updated the publish to MS Word option in the SAIDI/SAIFI calculator
The user can now publish a report that automatically populates the
correct dates and performance values for the preselected date.
</commit_message>
<xml_diff>
--- a/Data/Templates.xlsx
+++ b/Data/Templates.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="153">
   <si>
     <t>key_NETWORK_NAME</t>
   </si>
@@ -291,19 +291,7 @@
     <t>- Total assessed against target</t>
   </si>
   <si>
-    <t>YTD SAIDI Cap</t>
-  </si>
-  <si>
     <t>- Projected Incentive/Penalty</t>
-  </si>
-  <si>
-    <t>YTD SAIDI Collar</t>
-  </si>
-  <si>
-    <t>YTD SAIFI Cap</t>
-  </si>
-  <si>
-    <t>YTD SAIFI Collar</t>
   </si>
   <si>
     <t>The Power Company</t>
@@ -593,6 +581,81 @@
   </si>
   <si>
     <t>SAIFI (Average Number of Interruptions/ICP)</t>
+  </si>
+  <si>
+    <t>EOY SAIDI Cap</t>
+  </si>
+  <si>
+    <t>EOY SAIDI Collar</t>
+  </si>
+  <si>
+    <t>EOY SAIFI Cap</t>
+  </si>
+  <si>
+    <t>EOY SAIFI Collar</t>
+  </si>
+  <si>
+    <t>key_EIL_CC_REV_RISK</t>
+  </si>
+  <si>
+    <t>key_TPC_CC_REV_RISK</t>
+  </si>
+  <si>
+    <t>key_OJV_CC_REV_RISK</t>
+  </si>
+  <si>
+    <t>key_EIL_CC_SAIDI_TARGET</t>
+  </si>
+  <si>
+    <t>key_EIL_CC_SAIFI_TARGET</t>
+  </si>
+  <si>
+    <t>key_TPC_CC_SAIDI_TARGET</t>
+  </si>
+  <si>
+    <t>key_OJV_CC_SAIDI_TARGET</t>
+  </si>
+  <si>
+    <t>key_OJV_CC_SAIFI_TARGET</t>
+  </si>
+  <si>
+    <t>key_TPC_CC_SAIFI_TARGET</t>
+  </si>
+  <si>
+    <t>key_EIL_CC_SAIDI_CAP</t>
+  </si>
+  <si>
+    <t>key_EIL_CC_SAIDI_COLLAR</t>
+  </si>
+  <si>
+    <t>key_EIL_CC_SAIFI_COLLAR</t>
+  </si>
+  <si>
+    <t>key_EIL_CC_SAIFI_CAP</t>
+  </si>
+  <si>
+    <t>key_TPC_CC_SAIDI_CAP</t>
+  </si>
+  <si>
+    <t>key_TPC_CC_SAIDI_COLLAR</t>
+  </si>
+  <si>
+    <t>key_TPC_CC_SAIFI_CAP</t>
+  </si>
+  <si>
+    <t>key_TPC_CC_SAIFI_COLLAR</t>
+  </si>
+  <si>
+    <t>key_OJV_CC_SAIDI_CAP</t>
+  </si>
+  <si>
+    <t>key_OJV_CC_SAIDI_COLLAR</t>
+  </si>
+  <si>
+    <t>key_OJV_CC_SAIFI_CAP</t>
+  </si>
+  <si>
+    <t>key_OJV_CC_SAIFI_COLLAR</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1115,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1193,6 +1256,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1703,7 +1769,7 @@
   <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,10 +1816,10 @@
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="22" t="s">
@@ -1774,12 +1840,12 @@
         <v>35</v>
       </c>
       <c r="M3" s="25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="28"/>
@@ -1797,7 +1863,7 @@
         <v>26</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1806,12 +1872,12 @@
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="35"/>
       <c r="F5" s="34" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G5" s="34"/>
       <c r="H5" s="35"/>
@@ -1821,9 +1887,8 @@
       <c r="L5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="37">
-        <f>1%*13565*1000</f>
-        <v>135650</v>
+      <c r="M5" s="37" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1832,12 +1897,12 @@
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="35"/>
       <c r="F6" s="34" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="35"/>
@@ -1856,9 +1921,9 @@
         <f>SUM(C5:C6)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="51" t="e">
         <f>J7/12</f>
-        <v>2.0063238143920832</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="34">
@@ -1866,33 +1931,33 @@
         <v>0</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H7" s="35"/>
       <c r="I7" s="38" t="e">
         <f>F7-G7+J7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J7" s="45">
-        <v>24.075885772705</v>
+      <c r="J7" s="45" t="s">
+        <v>135</v>
       </c>
       <c r="K7" s="39"/>
       <c r="L7" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" s="1">
-        <v>31.126729965209901</v>
+        <v>128</v>
+      </c>
+      <c r="M7" s="59" t="s">
+        <v>141</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34"/>
@@ -1908,21 +1973,21 @@
       <c r="J8" s="34"/>
       <c r="K8" s="1"/>
       <c r="L8" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8" s="1">
-        <v>17.025041580200099</v>
+        <v>129</v>
+      </c>
+      <c r="M8" s="59" t="s">
+        <v>142</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="42" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="34"/>
@@ -1935,11 +2000,11 @@
       <c r="J9" s="36"/>
       <c r="K9" s="1"/>
       <c r="L9" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="M9" s="50">
+        <v>45</v>
+      </c>
+      <c r="M9" s="50" t="e">
         <f>0.5*M5/(M7-J7)</f>
-        <v>9619.415512272768</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1948,12 +2013,12 @@
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D10" s="45"/>
       <c r="E10" s="46"/>
       <c r="F10" s="34" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G10" s="45"/>
       <c r="H10" s="46"/>
@@ -1969,12 +2034,12 @@
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D11" s="45"/>
       <c r="E11" s="46"/>
       <c r="F11" s="34" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G11" s="38"/>
       <c r="H11" s="48"/>
@@ -1982,16 +2047,16 @@
       <c r="J11" s="49"/>
       <c r="K11" s="1"/>
       <c r="L11" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="1">
-        <v>0.77168273925781194</v>
+        <v>130</v>
+      </c>
+      <c r="M11" s="59" t="s">
+        <v>144</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2003,9 +2068,9 @@
         <f>SUM(C10:C11)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="51" t="e">
         <f>J12/12</f>
-        <v>4.9458478887875836E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E12" s="46"/>
       <c r="F12" s="38">
@@ -2013,33 +2078,33 @@
         <v>0</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H12" s="48"/>
       <c r="I12" s="38" t="e">
         <f>F12-G12+J12</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J12" s="45">
-        <v>0.59350174665451005</v>
+      <c r="J12" s="45" t="s">
+        <v>136</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="M12" s="1">
-        <v>0.41532078385353099</v>
+        <v>131</v>
+      </c>
+      <c r="M12" s="59" t="s">
+        <v>143</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34"/>
@@ -2055,16 +2120,16 @@
       <c r="J13" s="36"/>
       <c r="K13" s="1"/>
       <c r="L13" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="M13" s="50">
+        <v>46</v>
+      </c>
+      <c r="M13" s="50" t="e">
         <f>0.5*M5/(M11-J12)</f>
-        <v>380652.2738988442</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B14" s="43"/>
       <c r="C14" s="34"/>
@@ -2080,16 +2145,16 @@
     </row>
     <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="52" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="46"/>
       <c r="F15" s="52" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G15" s="45"/>
       <c r="H15" s="46"/>
@@ -2100,16 +2165,16 @@
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="52" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="46"/>
       <c r="F16" s="52" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G16" s="45"/>
       <c r="H16" s="46"/>
@@ -2120,16 +2185,16 @@
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="52" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="46"/>
       <c r="F17" s="52" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G17" s="45"/>
       <c r="H17" s="46"/>
@@ -2140,16 +2205,16 @@
     </row>
     <row r="18" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="52" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D18" s="45"/>
       <c r="E18" s="46"/>
       <c r="F18" s="52" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G18" s="45"/>
       <c r="H18" s="46"/>
@@ -2190,7 +2255,7 @@
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2211,10 +2276,10 @@
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E22" s="21"/>
       <c r="F22" s="22" t="s">
@@ -2235,13 +2300,13 @@
         <v>35</v>
       </c>
       <c r="M22" s="25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -2259,7 +2324,7 @@
         <v>26</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="O23" s="1"/>
     </row>
@@ -2269,12 +2334,12 @@
       </c>
       <c r="B24" s="33"/>
       <c r="C24" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D24" s="34"/>
       <c r="E24" s="35"/>
       <c r="F24" s="34" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G24" s="34"/>
       <c r="H24" s="35"/>
@@ -2284,8 +2349,8 @@
       <c r="L24" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="M24" s="53">
-        <v>438977</v>
+      <c r="M24" s="53" t="s">
+        <v>133</v>
       </c>
       <c r="O24" s="1"/>
     </row>
@@ -2295,12 +2360,12 @@
       </c>
       <c r="B25" s="33"/>
       <c r="C25" s="34" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D25" s="34"/>
       <c r="E25" s="35"/>
       <c r="F25" s="34" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G25" s="34"/>
       <c r="H25" s="35"/>
@@ -2319,9 +2384,9 @@
         <f>SUM(C24:C25)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="51">
+      <c r="D26" s="51" t="e">
         <f>J26/12</f>
-        <v>12.502338333333334</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E26" s="35"/>
       <c r="F26" s="34">
@@ -2329,33 +2394,33 @@
         <v>0</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H26" s="35"/>
       <c r="I26" s="34" t="e">
         <f>F26-G26+J26</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J26" s="45">
-        <v>150.02806000000001</v>
+      <c r="J26" s="45" t="s">
+        <v>137</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M26" s="1">
-        <v>165.66626439250879</v>
+        <v>128</v>
+      </c>
+      <c r="M26" s="59" t="s">
+        <v>145</v>
       </c>
       <c r="O26" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="33"/>
       <c r="C27" s="34"/>
@@ -2371,21 +2436,21 @@
       <c r="J27" s="34"/>
       <c r="K27" s="1"/>
       <c r="L27" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="M27" s="1">
-        <v>134.38985400061679</v>
+        <v>129</v>
+      </c>
+      <c r="M27" s="59" t="s">
+        <v>146</v>
       </c>
       <c r="O27" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="P27" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="42" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B28" s="43"/>
       <c r="C28" s="34"/>
@@ -2398,11 +2463,11 @@
       <c r="J28" s="36"/>
       <c r="K28" s="1"/>
       <c r="L28" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="M28" s="50">
+        <v>45</v>
+      </c>
+      <c r="M28" s="50" t="e">
         <f>0.5*M24/(M26-J26)</f>
-        <v>14035.402945950895</v>
+        <v>#VALUE!</v>
       </c>
       <c r="O28" s="1"/>
     </row>
@@ -2412,12 +2477,12 @@
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="46"/>
       <c r="F29" s="34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G29" s="45"/>
       <c r="H29" s="46"/>
@@ -2434,12 +2499,12 @@
       </c>
       <c r="B30" s="33"/>
       <c r="C30" s="34" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="46"/>
       <c r="F30" s="34" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G30" s="45"/>
       <c r="H30" s="46"/>
@@ -2447,16 +2512,16 @@
       <c r="J30" s="47"/>
       <c r="K30" s="1"/>
       <c r="L30" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M30" s="1">
-        <v>3.1582358015733725</v>
+        <v>130</v>
+      </c>
+      <c r="M30" s="59" t="s">
+        <v>147</v>
       </c>
       <c r="O30" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2468,9 +2533,9 @@
         <f>SUM(C29:C30)</f>
         <v>0</v>
       </c>
-      <c r="D31" s="45">
+      <c r="D31" s="45" t="e">
         <f>J31/12</f>
-        <v>0.23716833333333334</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E31" s="46"/>
       <c r="F31" s="45">
@@ -2478,33 +2543,33 @@
         <v>0</v>
       </c>
       <c r="G31" s="34" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H31" s="46"/>
       <c r="I31" s="45" t="e">
         <f>F31-G31+J31</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J31" s="45">
-        <v>2.8460200000000002</v>
+      <c r="J31" s="45" t="s">
+        <v>140</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="M31" s="1">
-        <v>2.5337967140967539</v>
+        <v>131</v>
+      </c>
+      <c r="M31" s="59" t="s">
+        <v>148</v>
       </c>
       <c r="O31" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="33"/>
       <c r="C32" s="34"/>
@@ -2520,16 +2585,16 @@
       <c r="J32" s="36"/>
       <c r="K32" s="1"/>
       <c r="L32" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="M32" s="50">
+        <v>46</v>
+      </c>
+      <c r="M32" s="50" t="e">
         <f>0.5*M24/(M30-J31)</f>
-        <v>703002.53508603771</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B33" s="43"/>
       <c r="C33" s="34"/>
@@ -2545,16 +2610,16 @@
     </row>
     <row r="34" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B34" s="33"/>
       <c r="C34" s="52" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D34" s="45"/>
       <c r="E34" s="46"/>
       <c r="F34" s="52" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G34" s="45"/>
       <c r="H34" s="46"/>
@@ -2565,16 +2630,16 @@
     </row>
     <row r="35" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B35" s="33"/>
       <c r="C35" s="52" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="46"/>
       <c r="F35" s="52" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G35" s="45"/>
       <c r="H35" s="46"/>
@@ -2585,16 +2650,16 @@
     </row>
     <row r="36" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B36" s="33"/>
       <c r="C36" s="52" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D36" s="45"/>
       <c r="E36" s="46"/>
       <c r="F36" s="52" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G36" s="45"/>
       <c r="H36" s="46"/>
@@ -2605,16 +2670,16 @@
     </row>
     <row r="37" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B37" s="33"/>
       <c r="C37" s="52" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D37" s="45"/>
       <c r="E37" s="46"/>
       <c r="F37" s="52" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G37" s="45"/>
       <c r="H37" s="46"/>
@@ -2655,7 +2720,7 @@
     </row>
     <row r="40" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2676,10 +2741,10 @@
       </c>
       <c r="B41" s="18"/>
       <c r="C41" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E41" s="21"/>
       <c r="F41" s="22" t="s">
@@ -2700,13 +2765,13 @@
         <v>35</v>
       </c>
       <c r="M41" s="25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="O41" s="1"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B42" s="27"/>
       <c r="C42" s="28"/>
@@ -2724,7 +2789,7 @@
         <v>26</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="O42" s="1"/>
     </row>
@@ -2734,12 +2799,12 @@
       </c>
       <c r="B43" s="33"/>
       <c r="C43" s="34" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D43" s="34"/>
       <c r="E43" s="35"/>
       <c r="F43" s="34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G43" s="34"/>
       <c r="H43" s="35"/>
@@ -2749,9 +2814,8 @@
       <c r="L43" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="M43" s="37">
-        <f>1%*24780*1000</f>
-        <v>247800</v>
+      <c r="M43" s="53" t="s">
+        <v>134</v>
       </c>
       <c r="O43" s="1"/>
     </row>
@@ -2761,12 +2825,12 @@
       </c>
       <c r="B44" s="33"/>
       <c r="C44" s="34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D44" s="34"/>
       <c r="E44" s="35"/>
       <c r="F44" s="34" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G44" s="34"/>
       <c r="H44" s="35"/>
@@ -2785,9 +2849,9 @@
         <f>SUM(C43:C44)</f>
         <v>0</v>
       </c>
-      <c r="D45" s="51">
+      <c r="D45" s="51" t="e">
         <f>J45/12</f>
-        <v>18.714778900146417</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E45" s="35"/>
       <c r="F45" s="34">
@@ -2795,33 +2859,33 @@
         <v>0</v>
       </c>
       <c r="G45" s="34" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H45" s="35"/>
       <c r="I45" s="34" t="e">
         <f>F45-G45+J45</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J45" s="45">
-        <v>224.57734680175699</v>
+      <c r="J45" s="45" t="s">
+        <v>138</v>
       </c>
       <c r="K45" s="1"/>
       <c r="L45" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M45" s="1">
-        <v>254.91531372070301</v>
+        <v>128</v>
+      </c>
+      <c r="M45" s="59" t="s">
+        <v>149</v>
       </c>
       <c r="O45" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" s="33"/>
       <c r="C46" s="34"/>
@@ -2837,21 +2901,21 @@
       <c r="J46" s="34"/>
       <c r="K46" s="1"/>
       <c r="L46" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="M46" s="1">
-        <v>194.23937988281199</v>
+        <v>129</v>
+      </c>
+      <c r="M46" s="59" t="s">
+        <v>150</v>
       </c>
       <c r="O46" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="42" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B47" s="43"/>
       <c r="C47" s="34"/>
@@ -2864,11 +2928,11 @@
       <c r="J47" s="36"/>
       <c r="K47" s="1"/>
       <c r="L47" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="M47" s="37">
+        <v>45</v>
+      </c>
+      <c r="M47" s="37" t="e">
         <f>0.5*M43/(M45-J45)</f>
-        <v>4083.9915321624471</v>
+        <v>#VALUE!</v>
       </c>
       <c r="O47" s="1"/>
     </row>
@@ -2878,12 +2942,12 @@
       </c>
       <c r="B48" s="33"/>
       <c r="C48" s="34" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D48" s="45"/>
       <c r="E48" s="46"/>
       <c r="F48" s="34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G48" s="45"/>
       <c r="H48" s="46"/>
@@ -2900,12 +2964,12 @@
       </c>
       <c r="B49" s="33"/>
       <c r="C49" s="34" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D49" s="45"/>
       <c r="E49" s="46"/>
       <c r="F49" s="34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G49" s="45"/>
       <c r="H49" s="46"/>
@@ -2913,16 +2977,16 @@
       <c r="J49" s="47"/>
       <c r="K49" s="1"/>
       <c r="L49" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M49" s="1">
-        <v>2.9273090362548801</v>
+        <v>130</v>
+      </c>
+      <c r="M49" s="59" t="s">
+        <v>151</v>
       </c>
       <c r="O49" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -2934,9 +2998,9 @@
         <f>SUM(C48:C49)</f>
         <v>0</v>
       </c>
-      <c r="D50" s="45">
+      <c r="D50" s="45" t="e">
         <f>J50/12</f>
-        <v>0.21032152573267582</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E50" s="46"/>
       <c r="F50" s="45">
@@ -2944,33 +3008,33 @@
         <v>0</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H50" s="46"/>
       <c r="I50" s="45" t="e">
         <f>F50-G50+J50</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J50" s="47">
-        <v>2.5238583087921098</v>
+      <c r="J50" s="45" t="s">
+        <v>139</v>
       </c>
       <c r="K50" s="1"/>
       <c r="L50" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="M50" s="1">
-        <v>2.1204075813293399</v>
+        <v>131</v>
+      </c>
+      <c r="M50" s="59" t="s">
+        <v>152</v>
       </c>
       <c r="O50" s="16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A51" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B51" s="33"/>
       <c r="C51" s="34"/>
@@ -2986,16 +3050,16 @@
       <c r="J51" s="36"/>
       <c r="K51" s="1"/>
       <c r="L51" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="M51" s="37">
+        <v>46</v>
+      </c>
+      <c r="M51" s="37" t="e">
         <f>0.5*M43/(M49-J50)</f>
-        <v>307100.69796920434</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="42" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B52" s="43"/>
       <c r="C52" s="34"/>
@@ -3009,16 +3073,16 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B53" s="33"/>
       <c r="C53" s="52" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D53" s="45"/>
       <c r="E53" s="46"/>
       <c r="F53" s="52" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G53" s="45"/>
       <c r="H53" s="46"/>
@@ -3027,16 +3091,16 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B54" s="33"/>
       <c r="C54" s="52" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D54" s="45"/>
       <c r="E54" s="46"/>
       <c r="F54" s="52" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G54" s="45"/>
       <c r="H54" s="46"/>
@@ -3045,16 +3109,16 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B55" s="33"/>
       <c r="C55" s="52" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D55" s="45"/>
       <c r="E55" s="46"/>
       <c r="F55" s="52" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G55" s="45"/>
       <c r="H55" s="46"/>
@@ -3063,16 +3127,16 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B56" s="33"/>
       <c r="C56" s="52" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D56" s="45"/>
       <c r="E56" s="46"/>
       <c r="F56" s="52" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G56" s="45"/>
       <c r="H56" s="46"/>

</xml_diff>

<commit_message>
Added new tables to the MS Word template
New tables include the number of faults (planned or unplanned) and the
the number of major event days. There are two new tables, containing the
same infomation for the current month and the year to date.
</commit_message>
<xml_diff>
--- a/Data/Templates.xlsx
+++ b/Data/Templates.xlsx
@@ -493,12 +493,6 @@
     <t>Raw</t>
   </si>
   <si>
-    <t>- Number of Unplanned Faults</t>
-  </si>
-  <si>
-    <t>- Number of Planned Faults</t>
-  </si>
-  <si>
     <t>key_EIL_RAW_MONTH_PLANNED</t>
   </si>
   <si>
@@ -656,6 +650,12 @@
   </si>
   <si>
     <t>key_OJV_CC_SAIFI_COLLAR</t>
+  </si>
+  <si>
+    <t>- Number of Planned Interruptions</t>
+  </si>
+  <si>
+    <t>- Number of Unplanned Interruptions</t>
   </si>
 </sst>
 </file>
@@ -1242,6 +1242,9 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1256,9 +1259,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1589,18 +1589,18 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="57"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -1768,9 +1768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1845,7 +1843,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="28"/>
@@ -1854,10 +1852,10 @@
       <c r="F4" s="28"/>
       <c r="G4" s="29"/>
       <c r="H4" s="31"/>
-      <c r="I4" s="57" t="s">
+      <c r="I4" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="58"/>
+      <c r="J4" s="59"/>
       <c r="K4" s="1"/>
       <c r="L4" s="16" t="s">
         <v>26</v>
@@ -1888,7 +1886,7 @@
         <v>24</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1939,14 +1937,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="J7" s="45" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K7" s="39"/>
       <c r="L7" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="M7" s="59" t="s">
-        <v>141</v>
+        <v>126</v>
+      </c>
+      <c r="M7" s="54" t="s">
+        <v>139</v>
       </c>
       <c r="O7" s="16" t="s">
         <v>43</v>
@@ -1973,10 +1971,10 @@
       <c r="J8" s="34"/>
       <c r="K8" s="1"/>
       <c r="L8" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="M8" s="59" t="s">
-        <v>142</v>
+        <v>127</v>
+      </c>
+      <c r="M8" s="54" t="s">
+        <v>140</v>
       </c>
       <c r="O8" s="16" t="s">
         <v>87</v>
@@ -1987,7 +1985,7 @@
     </row>
     <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="34"/>
@@ -2047,10 +2045,10 @@
       <c r="J11" s="49"/>
       <c r="K11" s="1"/>
       <c r="L11" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="M11" s="59" t="s">
-        <v>144</v>
+        <v>128</v>
+      </c>
+      <c r="M11" s="54" t="s">
+        <v>142</v>
       </c>
       <c r="O11" s="16" t="s">
         <v>44</v>
@@ -2086,14 +2084,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="J12" s="45" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="M12" s="59" t="s">
-        <v>143</v>
+        <v>129</v>
+      </c>
+      <c r="M12" s="54" t="s">
+        <v>141</v>
       </c>
       <c r="O12" s="16" t="s">
         <v>88</v>
@@ -2145,16 +2143,16 @@
     </row>
     <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="52" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="46"/>
       <c r="F15" s="52" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G15" s="45"/>
       <c r="H15" s="46"/>
@@ -2165,16 +2163,16 @@
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>98</v>
+        <v>152</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="52" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="46"/>
       <c r="F16" s="52" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G16" s="45"/>
       <c r="H16" s="46"/>
@@ -2185,16 +2183,16 @@
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="52" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="46"/>
       <c r="F17" s="52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G17" s="45"/>
       <c r="H17" s="46"/>
@@ -2205,16 +2203,16 @@
     </row>
     <row r="18" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="52" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D18" s="45"/>
       <c r="E18" s="46"/>
       <c r="F18" s="52" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G18" s="45"/>
       <c r="H18" s="46"/>
@@ -2306,7 +2304,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -2315,10 +2313,10 @@
       <c r="F23" s="28"/>
       <c r="G23" s="29"/>
       <c r="H23" s="31"/>
-      <c r="I23" s="57" t="s">
+      <c r="I23" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="J23" s="58"/>
+      <c r="J23" s="59"/>
       <c r="K23" s="1"/>
       <c r="L23" s="16" t="s">
         <v>26</v>
@@ -2350,7 +2348,7 @@
         <v>24</v>
       </c>
       <c r="M24" s="53" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="O24" s="1"/>
     </row>
@@ -2402,14 +2400,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="J26" s="45" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="M26" s="59" t="s">
-        <v>145</v>
+        <v>126</v>
+      </c>
+      <c r="M26" s="54" t="s">
+        <v>143</v>
       </c>
       <c r="O26" s="16" t="s">
         <v>43</v>
@@ -2436,10 +2434,10 @@
       <c r="J27" s="34"/>
       <c r="K27" s="1"/>
       <c r="L27" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="M27" s="59" t="s">
-        <v>146</v>
+        <v>127</v>
+      </c>
+      <c r="M27" s="54" t="s">
+        <v>144</v>
       </c>
       <c r="O27" s="16" t="s">
         <v>87</v>
@@ -2450,7 +2448,7 @@
     </row>
     <row r="28" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B28" s="43"/>
       <c r="C28" s="34"/>
@@ -2512,10 +2510,10 @@
       <c r="J30" s="47"/>
       <c r="K30" s="1"/>
       <c r="L30" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="M30" s="59" t="s">
-        <v>147</v>
+        <v>128</v>
+      </c>
+      <c r="M30" s="54" t="s">
+        <v>145</v>
       </c>
       <c r="O30" s="16" t="s">
         <v>44</v>
@@ -2551,14 +2549,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="J31" s="45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="M31" s="59" t="s">
-        <v>148</v>
+        <v>129</v>
+      </c>
+      <c r="M31" s="54" t="s">
+        <v>146</v>
       </c>
       <c r="O31" s="16" t="s">
         <v>88</v>
@@ -2610,16 +2608,16 @@
     </row>
     <row r="34" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="B34" s="33"/>
       <c r="C34" s="52" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D34" s="45"/>
       <c r="E34" s="46"/>
       <c r="F34" s="52" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G34" s="45"/>
       <c r="H34" s="46"/>
@@ -2630,16 +2628,16 @@
     </row>
     <row r="35" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
-        <v>98</v>
+        <v>152</v>
       </c>
       <c r="B35" s="33"/>
       <c r="C35" s="52" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="46"/>
       <c r="F35" s="52" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G35" s="45"/>
       <c r="H35" s="46"/>
@@ -2650,16 +2648,16 @@
     </row>
     <row r="36" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B36" s="33"/>
       <c r="C36" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D36" s="45"/>
       <c r="E36" s="46"/>
       <c r="F36" s="52" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G36" s="45"/>
       <c r="H36" s="46"/>
@@ -2670,16 +2668,16 @@
     </row>
     <row r="37" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B37" s="33"/>
       <c r="C37" s="52" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D37" s="45"/>
       <c r="E37" s="46"/>
       <c r="F37" s="52" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G37" s="45"/>
       <c r="H37" s="46"/>
@@ -2771,7 +2769,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B42" s="27"/>
       <c r="C42" s="28"/>
@@ -2780,10 +2778,10 @@
       <c r="F42" s="28"/>
       <c r="G42" s="29"/>
       <c r="H42" s="31"/>
-      <c r="I42" s="57" t="s">
+      <c r="I42" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="J42" s="58"/>
+      <c r="J42" s="59"/>
       <c r="K42" s="1"/>
       <c r="L42" s="16" t="s">
         <v>26</v>
@@ -2815,7 +2813,7 @@
         <v>24</v>
       </c>
       <c r="M43" s="53" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="O43" s="1"/>
     </row>
@@ -2867,14 +2865,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="J45" s="45" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K45" s="1"/>
       <c r="L45" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="M45" s="59" t="s">
-        <v>149</v>
+        <v>126</v>
+      </c>
+      <c r="M45" s="54" t="s">
+        <v>147</v>
       </c>
       <c r="O45" s="16" t="s">
         <v>43</v>
@@ -2901,10 +2899,10 @@
       <c r="J46" s="34"/>
       <c r="K46" s="1"/>
       <c r="L46" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="M46" s="59" t="s">
-        <v>150</v>
+        <v>127</v>
+      </c>
+      <c r="M46" s="54" t="s">
+        <v>148</v>
       </c>
       <c r="O46" s="16" t="s">
         <v>87</v>
@@ -2915,7 +2913,7 @@
     </row>
     <row r="47" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B47" s="43"/>
       <c r="C47" s="34"/>
@@ -2977,10 +2975,10 @@
       <c r="J49" s="47"/>
       <c r="K49" s="1"/>
       <c r="L49" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="M49" s="59" t="s">
-        <v>151</v>
+        <v>128</v>
+      </c>
+      <c r="M49" s="54" t="s">
+        <v>149</v>
       </c>
       <c r="O49" s="16" t="s">
         <v>44</v>
@@ -3016,14 +3014,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="J50" s="45" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K50" s="1"/>
       <c r="L50" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="M50" s="59" t="s">
-        <v>152</v>
+        <v>129</v>
+      </c>
+      <c r="M50" s="54" t="s">
+        <v>150</v>
       </c>
       <c r="O50" s="16" t="s">
         <v>88</v>
@@ -3073,16 +3071,16 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="B53" s="33"/>
       <c r="C53" s="52" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D53" s="45"/>
       <c r="E53" s="46"/>
       <c r="F53" s="52" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G53" s="45"/>
       <c r="H53" s="46"/>
@@ -3091,16 +3089,16 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
-        <v>98</v>
+        <v>152</v>
       </c>
       <c r="B54" s="33"/>
       <c r="C54" s="52" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D54" s="45"/>
       <c r="E54" s="46"/>
       <c r="F54" s="52" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G54" s="45"/>
       <c r="H54" s="46"/>
@@ -3109,16 +3107,16 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B55" s="33"/>
       <c r="C55" s="52" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D55" s="45"/>
       <c r="E55" s="46"/>
       <c r="F55" s="52" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G55" s="45"/>
       <c r="H55" s="46"/>
@@ -3127,16 +3125,16 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B56" s="33"/>
       <c r="C56" s="52" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D56" s="45"/>
       <c r="E56" s="46"/>
       <c r="F56" s="52" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G56" s="45"/>
       <c r="H56" s="46"/>

</xml_diff>